<commit_message>
ik snap t niet
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -494,17 +494,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WO_36</t>
+          <t>WO_11</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>VW_8</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>WO_53</t>
+          <t>WO_71</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -529,17 +529,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>WO_49</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>VW_5</t>
+          <t>VW_8</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>VW_3</t>
+          <t>WO_45</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -564,17 +564,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>VW_43</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>WO_32</t>
+          <t>WO_53</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>WO_41</t>
+          <t>WO_36</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -599,17 +599,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>VW_43</t>
+          <t>VW_15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>VW_62</t>
+          <t>WO_81</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>WO_13</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -634,7 +634,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>WO_23</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>VW_43</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -716,12 +716,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>WO_11</t>
+          <t>WO_21</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>WO_61</t>
+          <t>WO_81</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -735,7 +735,7 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -757,12 +757,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>WO_11</t>
+          <t>VW_32</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>VW_32</t>
+          <t>WO_69</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -798,26 +798,26 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>WO_11</t>
+          <t>VW_15</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>VW_23</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>VW_15</t>
+          <t>WO_24</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -839,26 +839,26 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>VW_31</t>
+          <t>VW_15</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>WO_24</t>
+          <t>VW_23</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>VW_15</t>
+          <t>VW_13</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -880,22 +880,22 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>VW_9</t>
+          <t>VW_18</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>VW_18</t>
+          <t>VW_27</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>WO_1</t>
+          <t>WO_26</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -921,22 +921,22 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>VW_18</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>VW_18</t>
+          <t>VW_27</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>WO_26</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -962,22 +962,22 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>WO_49</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>WO_81</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>VW_20</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>VW_8</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>WO_53</t>
-        </is>
-      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1003,22 +1003,22 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>WO_11</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>WO_81</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>VW_20</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>VW_62</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>VW_72</t>
-        </is>
-      </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1044,22 +1044,22 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>VW_27</t>
+          <t>VW_32</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>WO_61</t>
+          <t>VW_21</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>VW_21</t>
+          <t>VW_13</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1085,22 +1085,22 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>VW_20</t>
+          <t>VW_15</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>WO_45</t>
+          <t>VW_21</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>VW_21</t>
+          <t>WO_24</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1126,26 +1126,26 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>WO_49</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>VW_23</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>VW_8</t>
-        </is>
-      </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>VW_39</t>
+          <t>WO_45</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -1167,26 +1167,26 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>WO_49</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
           <t>VW_23</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>VW_35</t>
-        </is>
-      </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>WO_41</t>
+          <t>WO_45</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -1208,12 +1208,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>VW_43</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>WO_45</t>
+          <t>WO_85</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1249,12 +1249,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>WO_7</t>
+          <t>WO_33</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>VW_35</t>
+          <t>VW_12</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1290,22 +1290,22 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
+          <t>VW_32</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
           <t>VW_27</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>VW_18</t>
-        </is>
-      </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>WO_75</t>
+          <t>VW_13</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -1331,22 +1331,22 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t>WO_13</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>VW_27</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>VW_5</t>
-        </is>
-      </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>VW_21</t>
+          <t>WO_71</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -1358,40 +1358,40 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>VW_3_M_Huu</t>
+          <t>VW_31_M_Pau</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>VW_3</t>
+          <t>VW_31</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>WO_16</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>VW_12</t>
+          <t>VW_31</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>VW_3</t>
+          <t>VW_13</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -1399,40 +1399,40 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>VW_3_V_Cla</t>
+          <t>VW_31_V_Jan</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>VW_3</t>
+          <t>VW_31</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>VW_46</t>
+          <t>WO_79</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>VW_35</t>
+          <t>VW_31</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>VW_3</t>
+          <t>WO_71</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -1440,31 +1440,31 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>VW_31_M_Pau</t>
+          <t>VW_32_M_Mic</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>VW_31</t>
+          <t>VW_32</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>VW_31</t>
+          <t>VW_32</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>VW_12</t>
+          <t>VW_33</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>WO_53</t>
+          <t>VW_3</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1481,31 +1481,31 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>VW_31_V_Jan</t>
+          <t>VW_32_V_Wen</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>VW_31</t>
+          <t>VW_32</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>VW_31</t>
+          <t>VW_32</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>WO_77</t>
+          <t>VW_33</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>WO_50</t>
+          <t>VW_9</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1522,31 +1522,31 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>VW_32_M_Mic</t>
+          <t>VW_33_V_Het</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>VW_32</t>
+          <t>VW_33</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>VW_39</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>VW_32</t>
+          <t>VW_33</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>WO_36</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -1563,31 +1563,31 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>VW_32_V_Wen</t>
+          <t>VW_33_V_Tru</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>VW_32</t>
+          <t>VW_33</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>VW_46</t>
+          <t>VW_39</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>VW_32</t>
+          <t>VW_33</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>WO_49</t>
+          <t>VW_25</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1596,7 +1596,7 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
@@ -1604,40 +1604,40 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>VW_33_V_Het</t>
+          <t>VW_35_M_Roe</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>VW_33</t>
+          <t>VW_35</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>WO_40</t>
+          <t>VW_46</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>VW_70</t>
+          <t>VW_35</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>VW_33</t>
+          <t>VW_72</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
@@ -1645,40 +1645,40 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>VW_33_V_Tru</t>
+          <t>VW_35_V_Ros</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>VW_33</t>
+          <t>VW_35</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>WO_33</t>
+          <t>VW_46</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>WO_32</t>
+          <t>VW_35</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>VW_33</t>
+          <t>WO_71</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
@@ -1686,40 +1686,40 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>VW_35_M_Roe</t>
+          <t>VW_39_M_Bar</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>VW_35</t>
+          <t>VW_39</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>WO_85</t>
+          <t>VW_39</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>VW_35</t>
+          <t>WO_81</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>VW_25</t>
+          <t>VW_62</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
@@ -1727,40 +1727,40 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>VW_35_V_Ros</t>
+          <t>VW_39_V_Ann</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>VW_35</t>
+          <t>VW_39</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>WO_85</t>
+          <t>VW_39</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>VW_35</t>
+          <t>WO_61</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>WO_1</t>
+          <t>VW_9</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
@@ -1768,31 +1768,31 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>VW_39_M_Bar</t>
+          <t>VW_3_M_Huu</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>VW_39</t>
+          <t>VW_3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>WO_7</t>
+          <t>WO_11</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>VW_8</t>
+          <t>WO_27</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>VW_39</t>
+          <t>VW_3</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -1801,7 +1801,7 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
@@ -1809,31 +1809,31 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>VW_39_V_Ann</t>
+          <t>VW_3_V_Cla</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>VW_39</t>
+          <t>VW_3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>VW_46</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>VW_70</t>
+          <t>WO_27</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>VW_39</t>
+          <t>VW_3</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
@@ -1869,12 +1869,12 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>VW_70</t>
+          <t>WO_61</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>WO_20</t>
+          <t>VW_20</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1883,7 +1883,7 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -1910,12 +1910,12 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>WO_52</t>
+          <t>VW_33</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>WO_49</t>
+          <t>VW_20</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
@@ -1951,12 +1951,12 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>VW_70</t>
+          <t>VW_8</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>VW_3</t>
+          <t>VW_57</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -1965,7 +1965,7 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39">
@@ -1992,12 +1992,12 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>VW_12</t>
+          <t>WO_7</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>WO_53</t>
+          <t>VW_57</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2006,7 +2006,7 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40">
@@ -2014,36 +2014,36 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>VW_5_M_Car</t>
+          <t>VW_51_M_Coe</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>VW_5</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>WO_51</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>VW_5</t>
+          <t>WO_53</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>WO_55</t>
+          <t>VW_70</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -2055,36 +2055,36 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>VW_5_V_Jud</t>
+          <t>VW_51_V_Eli</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>VW_5</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>WO_51</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>VW_5</t>
+          <t>VW_33</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>WO_55</t>
+          <t>VW_20</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -2096,40 +2096,40 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>VW_51_M_Coe</t>
+          <t>VW_57_M_Lou</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>VW_57</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>VW_23</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>WO_87</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>WO_55</t>
+          <t>VW_57</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -2137,40 +2137,40 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>VW_51_V_Eli</t>
+          <t>VW_57_V_Ann</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>VW_57</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
+          <t>WO_41</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
           <t>VW_23</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>VW_51</t>
-        </is>
-      </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>WO_87</t>
+          <t>VW_57</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44">
@@ -2178,40 +2178,40 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>VW_57_M_Lou</t>
+          <t>VW_5_M_Car</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>VW_57</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>VW_57</t>
+          <t>VW_32</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>WO_38</t>
+          <t>WO_87</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>WO_87</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
@@ -2219,40 +2219,40 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>VW_57_V_Ann</t>
+          <t>VW_5_V_Jud</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>VW_57</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>VW_57</t>
+          <t>VW_32</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>WO_32</t>
+          <t>WO_40</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>WO_16</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
@@ -2260,40 +2260,40 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>VW_6_V_Len</t>
+          <t>VW_62_M_Rob</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>VW_6</t>
+          <t>VW_62</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>VW_6</t>
+          <t>WO_33</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>WO_45</t>
+          <t>WO_27</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>VW_25</t>
+          <t>VW_62</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
@@ -2301,11 +2301,11 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>VW_62_M_Rob</t>
+          <t>VW_62_V_Ale</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2315,22 +2315,22 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>VW_43</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
+          <t>WO_81</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
           <t>VW_62</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>VW_21</t>
-        </is>
-      </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -2342,52 +2342,46 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>VW_62_V_Ale</t>
+          <t>VW_68_M_Chr</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>VW_62</t>
+          <t>VW_68</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>WO_27</t>
+          <t>WO_20</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>VW_62</t>
+          <t>WO_51</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>WO_49</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Hoofd</t>
-        </is>
-      </c>
-      <c r="I48" t="n">
-        <v>6</v>
-      </c>
+          <t>WO_24</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>VW_68_M_Chr</t>
+          <t>VW_68_V_Mar</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2397,17 +2391,17 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>WO_23</t>
+          <t>WO_20</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>WO_71</t>
+          <t>WO_51</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>VW_33</t>
+          <t>WO_26</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
@@ -2418,35 +2412,41 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>VW_68_V_Mar</t>
+          <t>VW_6_V_Len</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>VW_68</t>
+          <t>VW_6</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>VW_20</t>
+          <t>WO_33</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>WO_71</t>
+          <t>VW_6</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>WO_75</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr"/>
+          <t>VW_25</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Hoofd</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2467,26 +2467,26 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>WO_51</t>
+          <t>WO_79</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
+          <t>VW_27</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
           <t>VW_70</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>WO_20</t>
-        </is>
-      </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52">
@@ -2508,26 +2508,26 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>WO_51</t>
+          <t>WO_79</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
+          <t>WO_53</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
           <t>VW_70</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>WO_41</t>
-        </is>
-      </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53">
@@ -2549,12 +2549,12 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>VW_46</t>
+          <t>VW_15</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>VW_8</t>
+          <t>WO_40</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2590,12 +2590,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>VW_31</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>WO_38</t>
+          <t>VW_8</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2631,7 +2631,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>WO_16</t>
+          <t>WO_26</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -2650,7 +2650,7 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>WO_40</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>VW_21</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -2691,7 +2691,7 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
@@ -2713,22 +2713,22 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
+          <t>VW_39</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>WO_40</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
           <t>VW_9</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>VW_5</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>WO_55</t>
-        </is>
-      </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -2754,22 +2754,22 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
+          <t>VW_32</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>WO_40</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
           <t>VW_9</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>VW_5</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>WO_75</t>
-        </is>
-      </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -2781,16 +2781,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>WO_1_M_And</t>
+          <t>WO_11_M_Bas</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>WO_1</t>
+          <t>WO_11</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2800,21 +2800,21 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>VW_21</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>WO_1</t>
+          <t>WO_52</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I59" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60">
@@ -2822,40 +2822,40 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>WO_1_V_Bir</t>
+          <t>WO_13_M_Lau</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>WO_1</t>
+          <t>WO_13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>WO_85</t>
+          <t>WO_13</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>VW_62</t>
+          <t>VW_35</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>WO_1</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61">
@@ -2863,31 +2863,31 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>WO_11_M_Bas</t>
+          <t>WO_13_V_Sim</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>WO_11</t>
+          <t>WO_13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>WO_11</t>
+          <t>WO_13</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>WO_38</t>
+          <t>WO_40</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>VW_3</t>
+          <t>WO_32</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -2896,7 +2896,7 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="62">
@@ -2904,36 +2904,36 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>WO_13_M_Lau</t>
+          <t>WO_16_M_Fre</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>WO_13</t>
+          <t>WO_16</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>WO_40</t>
+          <t>WO_16</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>VW_32</t>
+          <t>WO_85</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>WO_13</t>
+          <t>WO_52</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -2945,36 +2945,36 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>WO_13_V_Sim</t>
+          <t>WO_16_V_Lie</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>WO_13</t>
+          <t>WO_16</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>VW_20</t>
+          <t>WO_16</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
+          <t>WO_69</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
           <t>WO_52</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>WO_13</t>
-        </is>
-      </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -2986,31 +2986,31 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>WO_16_M_Fre</t>
+          <t>WO_1_M_And</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>WO_16</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>VW_57</t>
+          <t>WO_38</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>VW_32</t>
+          <t>VW_21</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>WO_16</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -3019,7 +3019,7 @@
         </is>
       </c>
       <c r="I64" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65">
@@ -3027,31 +3027,31 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>WO_16_V_Lie</t>
+          <t>WO_1_V_Bir</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>WO_16</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>VW_57</t>
+          <t>VW_46</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>VW_32</t>
+          <t>VW_23</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>WO_16</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -3060,7 +3060,7 @@
         </is>
       </c>
       <c r="I65" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66">
@@ -3082,22 +3082,22 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>VW_6</t>
+          <t>WO_20</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>VW_8</t>
+          <t>VW_35</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>WO_20</t>
+          <t>WO_75</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -3123,22 +3123,22 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>WO_27</t>
+          <t>WO_20</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>VW_12</t>
+          <t>VW_35</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>WO_20</t>
+          <t>WO_36</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -3169,12 +3169,12 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>WO_32</t>
+          <t>VW_23</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>VW_72</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -3183,7 +3183,7 @@
         </is>
       </c>
       <c r="I68" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
@@ -3210,12 +3210,12 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>WO_79</t>
+          <t>WO_27</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>WO_41</t>
+          <t>VW_20</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -3224,7 +3224,7 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
@@ -3251,12 +3251,12 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>VW_70</t>
+          <t>VW_31</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>WO_20</t>
+          <t>VW_9</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -3292,12 +3292,12 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>WO_77</t>
+          <t>VW_31</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>VW_15</t>
+          <t>VW_9</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -3328,26 +3328,26 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>WO_27</t>
+          <t>VW_43</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
+          <t>WO_55</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
           <t>WO_24</t>
         </is>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>VW_39</t>
-        </is>
-      </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I72" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73">
@@ -3369,26 +3369,26 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>WO_27</t>
+          <t>WO_21</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
+          <t>VW_35</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
           <t>WO_24</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>VW_39</t>
-        </is>
-      </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74">
@@ -3410,22 +3410,22 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>WO_85</t>
+          <t>VW_46</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
+          <t>VW_35</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
           <t>WO_26</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>WO_50</t>
-        </is>
-      </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -3451,22 +3451,22 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>VW_46</t>
+          <t>WO_41</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
+          <t>WO_53</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
           <t>WO_26</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>VW_39</t>
-        </is>
-      </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -3492,14 +3492,14 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
+          <t>WO_23</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
           <t>WO_27</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>WO_52</t>
-        </is>
-      </c>
       <c r="G76" t="inlineStr">
         <is>
           <t>VW_3</t>
@@ -3507,11 +3507,11 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
@@ -3533,14 +3533,14 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
+          <t>WO_21</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
           <t>WO_27</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>WO_79</t>
-        </is>
-      </c>
       <c r="G77" t="inlineStr">
         <is>
           <t>VW_3</t>
@@ -3548,11 +3548,11 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78">
@@ -3574,26 +3574,26 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>VW_6</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
+          <t>VW_12</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
           <t>WO_32</t>
         </is>
       </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>WO_87</t>
-        </is>
-      </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I78" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79">
@@ -3615,26 +3615,26 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>VW_9</t>
+          <t>WO_38</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
+          <t>VW_12</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
           <t>WO_32</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>WO_75</t>
-        </is>
-      </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80">
@@ -3656,17 +3656,17 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>VW_27</t>
+          <t>WO_13</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>WO_52</t>
+          <t>WO_55</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>VW_25</t>
+          <t>WO_32</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
@@ -3691,17 +3691,17 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>WO_40</t>
+          <t>WO_49</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>WO_55</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>WO_81</t>
+          <t>VW_13</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -3731,12 +3731,12 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>WO_32</t>
+          <t>WO_61</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>VW_15</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -3772,12 +3772,12 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>WO_77</t>
+          <t>WO_61</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>VW_15</t>
+          <t>WO_24</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -3808,26 +3808,26 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
+          <t>WO_38</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>VW_6</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
           <t>WO_36</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>WO_45</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>WO_87</t>
-        </is>
-      </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85">
@@ -3849,26 +3849,26 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
+          <t>WO_33</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>VW_6</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
           <t>WO_36</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>VW_12</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>WO_1</t>
-        </is>
-      </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86">
@@ -3890,26 +3890,26 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>VW_9</t>
+          <t>WO_38</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>WO_32</t>
+          <t>WO_87</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>WO_41</t>
+          <t>VW_25</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87">
@@ -3931,26 +3931,26 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>VW_27</t>
+          <t>WO_38</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>WO_38</t>
+          <t>WO_87</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>WO_41</t>
+          <t>WO_32</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I87" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
@@ -3972,22 +3972,22 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
+          <t>WO_13</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
           <t>WO_40</t>
         </is>
       </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>WO_32</t>
-        </is>
-      </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>VW_33</t>
+          <t>VW_3</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -4013,22 +4013,22 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
+          <t>WO_13</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
           <t>WO_40</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>WO_26</t>
-        </is>
-      </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>VW_15</t>
+          <t>VW_3</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -4054,26 +4054,26 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>VW_31</t>
+          <t>WO_41</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>WO_24</t>
+          <t>VW_21</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>WO_41</t>
+          <t>WO_1</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91">
@@ -4095,26 +4095,26 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>WO_36</t>
+          <t>WO_41</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>WO_24</t>
+          <t>VW_21</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>VW_13</t>
+          <t>WO_75</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I91" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92">
@@ -4136,22 +4136,22 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>VW_23</t>
+          <t>WO_49</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
+          <t>VW_31</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
           <t>WO_45</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>WO_13</t>
-        </is>
-      </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I92" t="n">
@@ -4177,22 +4177,22 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>WO_36</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
+          <t>VW_31</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
           <t>WO_45</t>
         </is>
       </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>WO_50</t>
-        </is>
-      </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I93" t="n">
@@ -4218,26 +4218,26 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
+          <t>WO_49</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>VW_31</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
           <t>VW_57</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>VW_32</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>WO_49</t>
-        </is>
-      </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I94" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95">
@@ -4259,26 +4259,26 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
+          <t>WO_49</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>VW_8</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
           <t>VW_57</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>VW_12</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>WO_49</t>
-        </is>
-      </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I95" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96">
@@ -4300,12 +4300,12 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>VW_23</t>
+          <t>VW_51</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>WO_77</t>
+          <t>VW_12</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -4341,12 +4341,12 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>VW_6</t>
+          <t>VW_43</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>WO_26</t>
+          <t>VW_12</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -4382,22 +4382,22 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
+          <t>VW_39</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
           <t>WO_51</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>VW_8</t>
-        </is>
-      </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>VW_15</t>
+          <t>WO_36</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I98" t="n">
@@ -4423,22 +4423,22 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
+          <t>VW_39</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
           <t>WO_51</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>VW_5</t>
-        </is>
-      </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>VW_21</t>
+          <t>VW_25</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I99" t="n">
@@ -4464,22 +4464,22 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>WO_69</t>
+          <t>VW_43</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
+          <t>WO_51</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
           <t>WO_52</t>
         </is>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>VW_72</t>
-        </is>
-      </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I100" t="n">
@@ -4505,22 +4505,22 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>WO_27</t>
+          <t>WO_23</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
+          <t>VW_23</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
           <t>WO_52</t>
         </is>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>VW_21</t>
-        </is>
-      </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I101" t="n">
@@ -4546,22 +4546,22 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>WO_36</t>
+          <t>WO_41</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>WO_26</t>
+          <t>WO_53</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>WO_53</t>
+          <t>WO_75</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I102" t="n">
@@ -4587,22 +4587,22 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>WO_36</t>
+          <t>WO_41</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>WO_26</t>
+          <t>WO_53</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>WO_53</t>
+          <t>WO_75</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I103" t="n">
@@ -4628,22 +4628,22 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>WO_69</t>
+          <t>WO_20</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>WO_71</t>
+          <t>WO_55</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>WO_55</t>
+          <t>VW_13</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I104" t="n">
@@ -4669,17 +4669,17 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
+          <t>VW_18</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
           <t>WO_7</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>VW_18</t>
-        </is>
-      </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>VW_13</t>
+          <t>WO_50</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -4704,12 +4704,12 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>WO_21</t>
+          <t>VW_18</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>VW_35</t>
+          <t>WO_7</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -4739,7 +4739,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>WO_40</t>
+          <t>WO_79</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -4749,7 +4749,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>WO_1</t>
+          <t>VW_62</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -4780,7 +4780,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>WO_7</t>
+          <t>WO_16</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -4790,7 +4790,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>WO_49</t>
+          <t>VW_62</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -4821,17 +4821,17 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>VW_9</t>
+          <t>WO_13</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>WO_71</t>
+          <t>WO_55</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>WO_16</t>
+          <t>VW_62</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
@@ -4856,17 +4856,17 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>WO_40</t>
+          <t>WO_13</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>VW_6</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>WO_49</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
@@ -4891,22 +4891,22 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
+          <t>VW_15</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
           <t>WO_69</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>VW_62</t>
-        </is>
-      </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>VW_39</t>
+          <t>WO_36</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I111" t="n">
@@ -4932,22 +4932,22 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
+          <t>VW_15</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
           <t>WO_69</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>WO_24</t>
-        </is>
-      </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>WO_16</t>
+          <t>WO_36</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I112" t="n">
@@ -4959,36 +4959,36 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>WO_7_M_San</t>
+          <t>WO_71_M_Kar</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>WO_7</t>
+          <t>WO_71</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>WO_7</t>
+          <t>WO_23</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>VW_18</t>
+          <t>VW_27</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>VW_13</t>
+          <t>WO_71</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I113" t="n">
@@ -5000,36 +5000,36 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>WO_7_V_Mon</t>
+          <t>WO_71_V_Mar</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>WO_7</t>
+          <t>WO_71</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>WO_7</t>
+          <t>WO_20</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>VW_18</t>
+          <t>WO_51</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>VW_13</t>
+          <t>WO_71</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I114" t="n">
@@ -5041,36 +5041,36 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>WO_71_M_Kar</t>
+          <t>WO_75_M_Jur</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>WO_71</t>
+          <t>WO_75</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>WO_23</t>
+          <t>WO_16</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>WO_71</t>
+          <t>WO_69</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>VW_33</t>
+          <t>WO_75</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I115" t="n">
@@ -5082,36 +5082,36 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>WO_71_V_Mar</t>
+          <t>WO_75_V_Deb</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>WO_71</t>
+          <t>WO_75</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>WO_23</t>
+          <t>WO_16</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>WO_71</t>
+          <t>WO_7</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>VW_33</t>
+          <t>WO_75</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Na</t>
         </is>
       </c>
       <c r="I116" t="n">
@@ -5123,40 +5123,40 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>WO_75_M_Jur</t>
+          <t>WO_77_M_Twa</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>WO_75</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>VW_31</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>VW_51</t>
+          <t>WO_40</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>WO_75</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I117" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118">
@@ -5164,40 +5164,40 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>WO_75_V_Deb</t>
+          <t>WO_77_V_Maa</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>WO_75</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>VW_43</t>
+          <t>WO_77</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>WO_79</t>
+          <t>WO_69</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>WO_75</t>
+          <t>VW_5</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I118" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119">
@@ -5205,36 +5205,36 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>WO_77_M_Twa</t>
+          <t>WO_79_M_Rob</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>WO_77</t>
+          <t>WO_79</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
+          <t>WO_79</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
           <t>WO_85</t>
         </is>
       </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>WO_77</t>
-        </is>
-      </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>VW_72</t>
+          <t>WO_45</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I119" t="n">
@@ -5246,36 +5246,36 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>WO_77_V_Maa</t>
+          <t>WO_79_V_Wie</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>WO_77</t>
+          <t>WO_79</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>WO_69</t>
+          <t>WO_79</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>WO_77</t>
+          <t>WO_85</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>WO_81</t>
+          <t>WO_52</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Hoofd</t>
+          <t>Voor</t>
         </is>
       </c>
       <c r="I120" t="n">
@@ -5287,31 +5287,31 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>WO_79_M_Rob</t>
+          <t>WO_7_M_San</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>WO_79</t>
+          <t>WO_7</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>WO_23</t>
+          <t>VW_18</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>WO_79</t>
+          <t>WO_7</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>VW_21</t>
+          <t>WO_50</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -5328,31 +5328,31 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>WO_79_V_Wie</t>
+          <t>WO_7_V_Mon</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>WO_79</t>
+          <t>WO_7</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>VW_20</t>
+          <t>VW_18</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>WO_79</t>
+          <t>WO_7</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>VW_39</t>
+          <t>WO_50</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
@@ -5383,26 +5383,26 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>WO_69</t>
+          <t>VW_39</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>VW_5</t>
+          <t>WO_81</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>WO_81</t>
+          <t>VW_70</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I123" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124">
@@ -5424,26 +5424,26 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>VW_23</t>
+          <t>VW_15</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>WO_24</t>
+          <t>WO_81</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>WO_81</t>
+          <t>VW_70</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I124" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125">
@@ -5465,26 +5465,26 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
+          <t>VW_51</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
           <t>WO_85</t>
         </is>
       </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>WO_79</t>
-        </is>
-      </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>VW_25</t>
+          <t>VW_70</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I125" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126">
@@ -5506,26 +5506,26 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
+          <t>WO_21</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
           <t>WO_85</t>
         </is>
       </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>WO_38</t>
-        </is>
-      </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>WO_81</t>
+          <t>WO_32</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>Voor</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I126" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127">
@@ -5547,22 +5547,22 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>WO_33</t>
+          <t>WO_38</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>WO_61</t>
+          <t>WO_87</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>WO_87</t>
+          <t>VW_72</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Na</t>
+          <t>Hoofd</t>
         </is>
       </c>
       <c r="I127" t="n">
@@ -5588,17 +5588,17 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>WO_33</t>
+          <t>WO_38</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>WO_24</t>
+          <t>VW_21</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>WO_13</t>
+          <t>VW_72</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
@@ -5623,17 +5623,17 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>WO_33</t>
+          <t>WO_38</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>WO_61</t>
+          <t>VW_21</t>
         </is>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>WO_13</t>
+          <t>VW_72</t>
         </is>
       </c>
       <c r="H129" t="inlineStr"/>

</xml_diff>